<commit_message>
Add parser for exel file, add discount column for dish model
</commit_message>
<xml_diff>
--- a/src/admin/Menu.xlsx
+++ b/src/admin/Menu.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Projects/PycharmProjects/examples/dishesApiProject/src/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E15110B-80DD-4A44-BF68-6C0E159A961C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5E22A1-7768-7441-BCF3-3C06CC1BF29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="14100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="260" yWindow="880" windowWidth="29660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Меню" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Меню</t>
   </si>
@@ -133,13 +133,34 @@
   </si>
   <si>
     <t>Нарезка из ветчины, колбасных колечек, нескольких сортов сыра и фруктов</t>
+  </si>
+  <si>
+    <t>№ меню</t>
+  </si>
+  <si>
+    <t>Название меню</t>
+  </si>
+  <si>
+    <t>Описание меню / Название подменю</t>
+  </si>
+  <si>
+    <t>Описание подменю / Название блюда</t>
+  </si>
+  <si>
+    <t>Описание блюда</t>
+  </si>
+  <si>
+    <t>Стоимость блюда</t>
+  </si>
+  <si>
+    <t>Скидка</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -148,20 +169,43 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Montserrat"/>
+      <charset val="204"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -184,27 +228,170 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,329 +611,356 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G1000"/>
+  <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="77.6640625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="1" max="1" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="86.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="35" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="1"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="14"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1">
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="1"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="13"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2">
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F4" s="7">
         <v>182.99</v>
       </c>
-      <c r="G3">
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="7">
+        <v>215.36</v>
+      </c>
+      <c r="G5" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="7">
+        <v>265.57</v>
+      </c>
+      <c r="G6" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="13"/>
     </row>
-    <row r="4" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2">
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="7">
+        <v>166.47</v>
+      </c>
+      <c r="G8" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6">
         <v>2</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="1">
-        <v>215.36</v>
-      </c>
-      <c r="G4">
+      <c r="D9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7">
+        <v>168.25</v>
+      </c>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="7">
+        <v>132.88</v>
+      </c>
+      <c r="G10" s="13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="7">
+        <v>2700.79</v>
+      </c>
+      <c r="G13" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2">
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6">
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3100.33</v>
+      </c>
+      <c r="G14" s="13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1">
-        <v>265.57</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
-      </c>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1850.42</v>
+      </c>
+      <c r="G15" s="13"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1">
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
+      <c r="C16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6">
+        <v>1</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="7">
+        <v>420.78</v>
+      </c>
+      <c r="G17" s="13">
         <v>10</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="1">
-        <v>166.47</v>
-      </c>
-      <c r="G7">
-        <v>15</v>
+    <row r="18" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6">
+        <v>2</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="7">
+        <v>440.11</v>
+      </c>
+      <c r="G18" s="13">
+        <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="1">
-        <v>168.25</v>
-      </c>
-      <c r="G8">
-        <v>20</v>
-      </c>
+    <row r="19" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6">
+        <v>3</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="7">
+        <v>520.08000000000004</v>
+      </c>
+      <c r="G19" s="13"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="1">
-        <v>132.88</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="2">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1">
-        <v>2700.79</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2">
-        <v>2</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3100.33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="2">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1850.42</v>
-      </c>
-      <c r="G14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="1">
-        <v>420.78</v>
-      </c>
-      <c r="G16">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="1">
-        <v>440.11</v>
-      </c>
-      <c r="G17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1">
-        <v>3</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="1">
-        <v>520.08000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1728,6 +1942,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add background task with data synchronization from an excel file
</commit_message>
<xml_diff>
--- a/src/admin/Menu.xlsx
+++ b/src/admin/Menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Projects/PycharmProjects/examples/dishesApiProject/src/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5E22A1-7768-7441-BCF3-3C06CC1BF29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FA9B69-F8F4-774D-BBF2-56D294AA14F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="880" windowWidth="29660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="920" windowWidth="29660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Меню" sheetId="1" r:id="rId1"/>
@@ -614,7 +614,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="G19" sqref="A2:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Add out discount price
</commit_message>
<xml_diff>
--- a/src/admin/Menu.xlsx
+++ b/src/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Projects/PycharmProjects/examples/dishesApiProject/src/admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FA9B69-F8F4-774D-BBF2-56D294AA14F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A9F8BC-D1A7-E049-B548-DE993A62A103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="660" yWindow="920" windowWidth="29660" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:G1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="A2:G19"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>